<commit_message>
End of night, version 2 of Game score is working in notbook
</commit_message>
<xml_diff>
--- a/data/Game_Score/Nov_11_Michigan State_GAME_SCORES.xlsx
+++ b/data/Game_Score/Nov_11_Michigan State_GAME_SCORES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\college_hockey\data\Game_Score\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922F5464-4AD6-4FC8-A5D6-5A72B5AC9D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A4654F-33FA-45E1-BE41-C223251D829D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-1020" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Michigan State_GAME_SCORES" sheetId="1" r:id="rId1"/>
@@ -961,16 +961,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1019,6 +1019,45 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="23">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="2" tint="-0.89999084444715716"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1094,45 +1133,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="2" tint="-0.89999084444715716"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1644,8 +1644,8 @@
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14" dataDxfId="6">
       <calculatedColumnFormula>SUM(D4:M4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="5">
-      <calculatedColumnFormula>AVERAGEIF(D4:M4, "&lt;&gt;0")</calculatedColumnFormula>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGEIF(B4:M4, "&lt;&gt;0")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1955,7 +1955,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,30 +1975,30 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="24" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="24" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="25"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="9" t="s">
         <v>29</v>
       </c>
@@ -2098,8 +2098,8 @@
         <v>13.2699836541954</v>
       </c>
       <c r="O4" s="12">
-        <f t="shared" ref="O4:O27" si="1">AVERAGEIF(D4:M4, "&lt;&gt;0")</f>
-        <v>1.3269983654195401</v>
+        <f t="shared" ref="O4:O27" si="1">AVERAGEIF(B4:M4, "&lt;&gt;0")</f>
+        <v>1.260831971182949</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="O5" s="12">
         <f t="shared" si="1"/>
-        <v>1.240999455139846</v>
+        <v>1.1866657585664107</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="O6" s="12">
         <f t="shared" si="1"/>
-        <v>1.0964956411187785</v>
+        <v>1.0420797009323153</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="O7" s="12">
         <f t="shared" si="1"/>
-        <v>1.0759994551398468</v>
+        <v>1.0179162126165389</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2295,7 +2295,7 @@
       </c>
       <c r="O8" s="12">
         <f t="shared" si="1"/>
-        <v>1.0199989102796942</v>
+        <v>1.1445819711829508</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="O9" s="12">
         <f t="shared" si="1"/>
-        <v>0.92749945513984655</v>
+        <v>0.95291621261653792</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="O10" s="12">
         <f t="shared" si="1"/>
-        <v>0.88699891027969269</v>
+        <v>0.97541530451628355</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="O11" s="12">
         <f t="shared" si="1"/>
-        <v>0.79428493591406568</v>
+        <v>0.83444383904427311</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="O12" s="12">
         <f t="shared" si="1"/>
-        <v>0.79374727569923575</v>
+        <v>0.82833060903256872</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="O13" s="12">
         <f t="shared" si="1"/>
-        <v>0.79111050571094021</v>
+        <v>0.84863586830894999</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="O14" s="12">
         <f t="shared" si="1"/>
-        <v>0.72099836541954165</v>
+        <v>0.91791530451628489</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="O15" s="12">
         <f t="shared" si="1"/>
-        <v>0.67666606126649709</v>
+        <v>0.60818132285440651</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="O16" s="12">
         <f t="shared" si="1"/>
-        <v>0.61949727569923674</v>
+        <v>0.69166439641602995</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="O17" s="12">
         <f t="shared" si="1"/>
-        <v>0.59285636448549628</v>
+        <v>0.54444383904427474</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2785,7 +2785,7 @@
       </c>
       <c r="O18" s="12">
         <f t="shared" si="1"/>
-        <v>0.57777596157726918</v>
+        <v>0.59999851401776549</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="O19" s="12">
         <f t="shared" si="1"/>
-        <v>0.55624931892480889</v>
+        <v>0.62149945513984695</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="O20" s="12">
         <f t="shared" si="1"/>
-        <v>0.52099673083908338</v>
+        <v>0.59714052202791668</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="O21" s="12">
         <f t="shared" si="1"/>
-        <v>0.50199673083908414</v>
+        <v>0.56041348831577631</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="O23" s="12">
         <f t="shared" si="1"/>
-        <v>0.45499455139847345</v>
+        <v>0.54562023247366442</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="O28" s="4">
         <f t="shared" si="2"/>
-        <v>16.299910456269906</v>
+        <v>16.902440708784674</v>
       </c>
     </row>
   </sheetData>
@@ -3308,7 +3308,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A27">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3343,7 +3343,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2 D2 F2 H2 J2 L2 N2:O2">
-    <cfRule type="cellIs" dxfId="3" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3368,7 +3368,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:M27">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3403,7 +3403,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N27">
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3448,7 +3448,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O27">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>